<commit_message>
Started to mess with file output
</commit_message>
<xml_diff>
--- a/resources/test-cube.xlsx
+++ b/resources/test-cube.xlsx
@@ -9,17 +9,18 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1890" yWindow="0" windowWidth="20880" windowHeight="8415" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2835" yWindow="0" windowWidth="20880" windowHeight="8415" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="test-cube" sheetId="1" r:id="rId1"/>
+    <sheet name="First Try" sheetId="1" r:id="rId1"/>
+    <sheet name="Second Try" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="171027"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>d</t>
   </si>
@@ -28,6 +29,21 @@
   </si>
   <si>
     <t>Radians</t>
+  </si>
+  <si>
+    <t>-1 -1 -1 1</t>
+  </si>
+  <si>
+    <t>1 -1 -1 1</t>
+  </si>
+  <si>
+    <t>1 -1 1 1</t>
+  </si>
+  <si>
+    <t>-1 1 0.999999 1</t>
+  </si>
+  <si>
+    <t>-0.999999 1 -1 1</t>
   </si>
 </sst>
 </file>
@@ -641,7 +657,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>'test-cube'!$B$17:$Y$17</c:f>
+              <c:f>'First Try'!$B$17:$Y$17</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="24"/>
@@ -722,7 +738,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'test-cube'!$B$18:$Y$18</c:f>
+              <c:f>'First Try'!$B$18:$Y$18</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="24"/>
@@ -1891,8 +1907,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:Z19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Z21" sqref="Z21"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="Z19" sqref="B17:Z19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2928,4 +2944,44 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{34819B32-8337-4201-A5E3-BA0BDF716277}">
+  <dimension ref="B2:B6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8:E12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="2" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>